<commit_message>
[ADD] cleaning data and transform data to index out of ten
</commit_message>
<xml_diff>
--- a/kkhj_happinessPerceptionReality/data/criminality2021.xlsx
+++ b/kkhj_happinessPerceptionReality/data/criminality2021.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\S8\PYBD\crime &amp; safety\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\S8\PYBD\delta\kkhj_happinessPerceptionReality\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0502B7F-B33A-4F38-A0B8-C8D414EE5FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA13D7E-9453-4141-B274-80E76EAB3F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2334" yWindow="672" windowWidth="17280" windowHeight="10074" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
   <si>
     <t>Rank</t>
   </si>
@@ -442,9 +442,6 @@
   </si>
   <si>
     <t>Qatar</t>
-  </si>
-  <si>
-    <t>https://www.numbeo.com/crime/rankings_by_country.jsp?title=2021</t>
   </si>
 </sst>
 </file>
@@ -827,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E136"/>
+  <dimension ref="A1:D136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -841,7 +838,7 @@
     <col min="4" max="4" width="15.5234375" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" ht="17.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -854,11 +851,8 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -872,7 +866,7 @@
         <v>15.75</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -886,7 +880,7 @@
         <v>19.760000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -900,7 +894,7 @@
         <v>22.93</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -914,7 +908,7 @@
         <v>23.63</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -928,7 +922,7 @@
         <v>25.22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -942,7 +936,7 @@
         <v>29.05</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -956,7 +950,7 @@
         <v>31.18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -970,7 +964,7 @@
         <v>31.26</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -984,7 +978,7 @@
         <v>31.91</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -998,7 +992,7 @@
         <v>32.15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1012,7 +1006,7 @@
         <v>32.47</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1026,7 +1020,7 @@
         <v>33.369999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1040,7 +1034,7 @@
         <v>33.39</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1054,7 +1048,7 @@
         <v>34.11</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2">
         <v>15</v>
       </c>

</xml_diff>